<commit_message>
Revert "Kamo bug fix for removal of LA"
</commit_message>
<xml_diff>
--- a/ILR_TestSuite/MIP UAT Test Scenarios/TestData.xlsx
+++ b/ILR_TestSuite/MIP UAT Test Scenarios/TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G992127\Documents\GitHub\ILR_TestSuite\ILR_TestSuite\MIP UAT Test Scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G992107\Documents\GitHub\ILR_TestSuite\ILR_TestSuite\MIP UAT Test Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC017EE9-B71D-4175-A884-3CA543498B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E40148-F547-4E6E-9EF5-6913A1CCE660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1681,11 +1681,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{122D3D24-972A-41AA-875A-C35A49A85BBB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{122D3D24-972A-41AA-875A-C35A49A85BBB}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="62" zoomScaleNormal="62" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1701,7 +1701,7 @@
     <col min="9" max="9" width="24.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row spans="1:9" s="1" customFormat="1" ht="18.5" x14ac:dyDescent="0.45" outlineLevel="0" r="1">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>11</v>
       </c>
     </row>
-    <row spans="1:9" ht="58" x14ac:dyDescent="0.35" outlineLevel="0" r="2">
+    <row r="2" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="45" t="s">
         <v>89</v>
       </c>
@@ -1753,7 +1753,7 @@
       <c r="H2" s="38"/>
       <c r="I2" s="31"/>
     </row>
-    <row spans="1:9" x14ac:dyDescent="0.35" outlineLevel="0" r="3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="45" t="s">
         <v>91</v>
       </c>
@@ -1770,7 +1770,7 @@
       <c r="H3" s="38"/>
       <c r="I3" s="31"/>
     </row>
-    <row spans="1:9" ht="43.5" x14ac:dyDescent="0.35" outlineLevel="0" r="4">
+    <row r="4" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="45" t="s">
         <v>91</v>
       </c>
@@ -1793,7 +1793,7 @@
       <c r="H4" s="38"/>
       <c r="I4" s="31"/>
     </row>
-    <row spans="1:9" ht="43.5" x14ac:dyDescent="0.35" outlineLevel="0" r="5">
+    <row r="5" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="45" t="s">
         <v>88</v>
       </c>
@@ -1816,7 +1816,7 @@
       <c r="H5" s="38"/>
       <c r="I5" s="31"/>
     </row>
-    <row spans="1:9" ht="29" x14ac:dyDescent="0.35" outlineLevel="0" r="6">
+    <row r="6" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="45" t="s">
         <v>84</v>
       </c>
@@ -1839,7 +1839,7 @@
       <c r="H6" s="38"/>
       <c r="I6" s="31"/>
     </row>
-    <row spans="1:9" ht="43.5" x14ac:dyDescent="0.35" outlineLevel="0" r="7">
+    <row r="7" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="45" t="s">
         <v>84</v>
       </c>
@@ -1862,7 +1862,7 @@
       <c r="H7" s="39"/>
       <c r="I7" s="40"/>
     </row>
-    <row spans="1:9" x14ac:dyDescent="0.35" outlineLevel="0" r="8">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="45"/>
       <c r="B8" s="45"/>
       <c r="C8" s="45"/>
@@ -1873,7 +1873,7 @@
       <c r="H8" s="39"/>
       <c r="I8" s="40"/>
     </row>
-    <row spans="1:9" x14ac:dyDescent="0.35" outlineLevel="0" r="9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="45" t="s">
         <v>197</v>
       </c>
@@ -1890,7 +1890,7 @@
       <c r="H9" s="39"/>
       <c r="I9" s="41"/>
     </row>
-    <row spans="1:9" ht="43.5" x14ac:dyDescent="0.35" outlineLevel="0" r="10">
+    <row r="10" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="45" t="s">
         <v>208</v>
       </c>
@@ -1913,7 +1913,7 @@
       <c r="H10" s="39"/>
       <c r="I10" s="41"/>
     </row>
-    <row spans="1:9" ht="87" x14ac:dyDescent="0.35" outlineLevel="0" r="11">
+    <row r="11" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A11" s="46" t="s">
         <v>93</v>
       </c>
@@ -1936,7 +1936,7 @@
       <c r="H11" s="39"/>
       <c r="I11" s="41"/>
     </row>
-    <row spans="1:9" ht="29" x14ac:dyDescent="0.35" outlineLevel="0" r="12">
+    <row r="12" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="49" t="s">
         <v>95</v>
       </c>
@@ -1959,7 +1959,7 @@
       <c r="H12" s="43"/>
       <c r="I12" s="44"/>
     </row>
-    <row spans="1:9" ht="29" x14ac:dyDescent="0.35" outlineLevel="0" r="13">
+    <row r="13" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="49" t="s">
         <v>197</v>
       </c>
@@ -1971,18 +1971,10 @@
       <c r="E13" s="49"/>
       <c r="F13" s="49"/>
       <c r="G13" s="42"/>
-      <c r="H13" s="43" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="I13" s="44" t="inlineStr">
-        <is>
-          <t>07/01/2022 10:21:51</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:9" x14ac:dyDescent="0.35" outlineLevel="0" r="14">
+      <c r="H13" s="43"/>
+      <c r="I13" s="44"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="50"/>
       <c r="B14" s="50"/>
       <c r="C14" s="51"/>

</xml_diff>

<commit_message>
Post dated upgrades and downgrades
</commit_message>
<xml_diff>
--- a/ILR_TestSuite/MIP UAT Test Scenarios/TestData.xlsx
+++ b/ILR_TestSuite/MIP UAT Test Scenarios/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\E697642\Documents\GitHub\ILR_TestSuite\ILR_TestSuite\MIP UAT Test Scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G992127\Documents\GitHub\ILR_TestSuite\ILR_TestSuite\MIP UAT Test Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37CF4179-38F1-4E42-A9A1-E916C3A80B66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74371C28-A856-4C6C-975F-1A0EE33D6D44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Policy-Servicing" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="239">
   <si>
     <t>Policy No</t>
   </si>
@@ -738,6 +738,30 @@
   </si>
   <si>
     <t>10/01/2022 14:59:00</t>
+  </si>
+  <si>
+    <t>PostDatedUpgrade</t>
+  </si>
+  <si>
+    <t>Upgrade benefits starting from next month</t>
+  </si>
+  <si>
+    <t>PostDatedDowngrade</t>
+  </si>
+  <si>
+    <t>Downgrade benefits starting from next month</t>
+  </si>
+  <si>
+    <t>SS11111122</t>
+  </si>
+  <si>
+    <t>SS40244230</t>
+  </si>
+  <si>
+    <t>11/01/2022 13:27:04</t>
+  </si>
+  <si>
+    <t>11/01/2022 13:11:27</t>
   </si>
 </sst>
 </file>
@@ -1739,10 +1763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{122D3D24-972A-41AA-875A-C35A49A85BBB}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2112,6 +2136,46 @@
       </c>
       <c r="I16" s="55" t="s">
         <v>230</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="49" t="s">
+        <v>235</v>
+      </c>
+      <c r="B17" t="s">
+        <v>231</v>
+      </c>
+      <c r="C17" t="s">
+        <v>232</v>
+      </c>
+      <c r="E17" s="49">
+        <v>300</v>
+      </c>
+      <c r="H17" s="55" t="s">
+        <v>227</v>
+      </c>
+      <c r="I17" s="55" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="49" t="s">
+        <v>236</v>
+      </c>
+      <c r="B18" t="s">
+        <v>233</v>
+      </c>
+      <c r="C18" t="s">
+        <v>234</v>
+      </c>
+      <c r="E18" s="49">
+        <v>300</v>
+      </c>
+      <c r="H18" s="55" t="s">
+        <v>227</v>
+      </c>
+      <c r="I18" s="55" t="s">
+        <v>238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
80%  log function coverage
</commit_message>
<xml_diff>
--- a/ILR_TestSuite/MIP UAT Test Scenarios/TestData.xlsx
+++ b/ILR_TestSuite/MIP UAT Test Scenarios/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G992127\Documents\GitHub\ILR_TestSuite\ILR_TestSuite\MIP UAT Test Scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G992107\Documents\GitHub\ILR_TestSuite\ILR_TestSuite\MIP UAT Test Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015198C1-DE4B-4DD7-9209-8D602D1CE56E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F620813-0DAD-4A3B-8489-C76C23D7C04D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Policy-Servicing" sheetId="2" r:id="rId1"/>
@@ -18,10 +18,11 @@
     <sheet name="Serenity_Premium" sheetId="4" r:id="rId3"/>
     <sheet name="Dropdown" sheetId="8" r:id="rId4"/>
     <sheet name="ChangeBeneData" sheetId="3" r:id="rId5"/>
-    <sheet name="Safrican_Just_Funeral" sheetId="5" r:id="rId6"/>
-    <sheet name="AddaLife" sheetId="9" r:id="rId7"/>
-    <sheet name="AddRolePlayer" sheetId="7" r:id="rId8"/>
-    <sheet name="AddRoleNext_month" sheetId="10" r:id="rId9"/>
+    <sheet name="CollectionM" sheetId="11" r:id="rId6"/>
+    <sheet name="Safrican_Just_Funeral" sheetId="5" r:id="rId7"/>
+    <sheet name="AddaLife" sheetId="9" r:id="rId8"/>
+    <sheet name="AddRolePlayer" sheetId="7" r:id="rId9"/>
+    <sheet name="AddRoleNext_month" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ChangeLifeData!$A$1:$F$2</definedName>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="249">
   <si>
     <t>Policy No</t>
   </si>
@@ -701,94 +702,97 @@
     <t>SS03245765</t>
   </si>
   <si>
-    <t>SS03245767</t>
-  </si>
-  <si>
     <t>SS03945701</t>
   </si>
   <si>
-    <t>0010229256085</t>
-  </si>
-  <si>
-    <t>2000/10/22</t>
-  </si>
-  <si>
-    <t>Zama</t>
-  </si>
-  <si>
     <t>Xulu</t>
   </si>
   <si>
-    <t>Z</t>
-  </si>
-  <si>
-    <t>SS11100099</t>
-  </si>
-  <si>
-    <t>SS03945702</t>
-  </si>
-  <si>
-    <t>0008089378080</t>
-  </si>
-  <si>
-    <t>SS11100699</t>
-  </si>
-  <si>
-    <t>0008087969088</t>
+    <t>SS11100095</t>
+  </si>
+  <si>
+    <t>SS03945704</t>
+  </si>
+  <si>
+    <t>SS03945705</t>
+  </si>
+  <si>
+    <t>0009285425089</t>
+  </si>
+  <si>
+    <t>2000/09/28</t>
+  </si>
+  <si>
+    <t>Linda</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>SS11100619</t>
+  </si>
+  <si>
+    <t>SS11100629</t>
+  </si>
+  <si>
+    <t>0008085568080</t>
+  </si>
+  <si>
+    <t>0008087370089</t>
   </si>
   <si>
     <t>Passed</t>
   </si>
   <si>
-    <t>13/01/2022 12:40:30</t>
-  </si>
-  <si>
-    <t>13/01/2022 12:43:34</t>
-  </si>
-  <si>
-    <t>13/01/2022 12:56:22</t>
-  </si>
-  <si>
-    <t>13/01/2022 12:58:51</t>
-  </si>
-  <si>
-    <t>SS11100095</t>
-  </si>
-  <si>
-    <t>13/01/2022 14:43:20</t>
-  </si>
-  <si>
-    <t>13/01/2022 14:33:05</t>
-  </si>
-  <si>
-    <t>13/01/2022 14:31:00</t>
-  </si>
-  <si>
-    <t>13/01/2022 14:44:28</t>
+    <t>13/01/2022 16:04:59</t>
+  </si>
+  <si>
+    <t>13/01/2022 16:07:02</t>
+  </si>
+  <si>
+    <t>13/01/2022 16:11:40</t>
+  </si>
+  <si>
+    <t>13/01/2022 16:13:35</t>
+  </si>
+  <si>
+    <t>13/01/2022 16:44:45</t>
+  </si>
+  <si>
+    <t>13/01/2022 16:42:56</t>
+  </si>
+  <si>
+    <t>13/01/2022 16:41:19</t>
+  </si>
+  <si>
+    <t>13/01/2022 16:46:09</t>
+  </si>
+  <si>
+    <t>13/01/2022 16:39:09</t>
+  </si>
+  <si>
+    <t>13/01/2022 16:55:34</t>
+  </si>
+  <si>
+    <t>13/01/2022 16:56:59</t>
   </si>
   <si>
     <t>Failed</t>
   </si>
   <si>
-    <t>13/01/2022 14:36:19</t>
-  </si>
-  <si>
-    <t>13/01/2022 14:48:59</t>
-  </si>
-  <si>
-    <t>13/01/2022 14:27:48</t>
-  </si>
-  <si>
-    <t>13/01/2022 14:46:45</t>
-  </si>
-  <si>
-    <t>13/01/2022 14:34:41</t>
-  </si>
-  <si>
-    <t>13/01/2022 14:20:33</t>
-  </si>
-  <si>
-    <t>13/01/2022 14:14:46</t>
+    <t>13/01/2022 17:16:30</t>
+  </si>
+  <si>
+    <t>13/01/2022 17:00:20</t>
+  </si>
+  <si>
+    <t>13/01/2022 16:58:17</t>
+  </si>
+  <si>
+    <t>employee_number1</t>
+  </si>
+  <si>
+    <t>employee_number2</t>
   </si>
 </sst>
 </file>
@@ -967,7 +971,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1069,6 +1073,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1776,18 +1783,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{122D3D24-972A-41AA-875A-C35A49A85BBB}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.6328125" customWidth="1"/>
-    <col min="2" max="2" width="27.453125" customWidth="1"/>
+    <col min="2" max="2" width="35.1796875" customWidth="1"/>
     <col min="3" max="3" width="43.36328125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.6328125" style="4" customWidth="1"/>
     <col min="5" max="5" width="16.36328125" customWidth="1"/>
-    <col min="6" max="6" width="22.1796875" customWidth="1"/>
+    <col min="6" max="6" width="25.1796875" customWidth="1"/>
     <col min="7" max="7" width="17.81640625" customWidth="1"/>
     <col min="8" max="8" width="16.1796875" customWidth="1"/>
     <col min="9" max="9" width="24.81640625" customWidth="1"/>
@@ -1843,10 +1850,10 @@
       </c>
       <c r="G2" s="49"/>
       <c r="H2" s="34" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="I2" s="27" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -1864,10 +1871,10 @@
       <c r="F3" s="38"/>
       <c r="G3" s="49"/>
       <c r="H3" s="34" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="I3" s="27" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
@@ -1891,10 +1898,10 @@
       </c>
       <c r="G4" s="49"/>
       <c r="H4" s="34" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="I4" s="27" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
@@ -1918,15 +1925,15 @@
       </c>
       <c r="G5" s="49"/>
       <c r="H5" s="34" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="38" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B6" s="38" t="s">
         <v>96</v>
@@ -1949,7 +1956,7 @@
     </row>
     <row r="7" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="38" t="s">
-        <v>218</v>
+        <v>90</v>
       </c>
       <c r="B7" s="38" t="s">
         <v>83</v>
@@ -1968,15 +1975,15 @@
       </c>
       <c r="G7" s="49"/>
       <c r="H7" s="35" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="I7" s="36" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="38" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B8" s="38" t="s">
         <v>89</v>
@@ -1991,15 +1998,15 @@
       <c r="F8" s="38"/>
       <c r="G8" s="49"/>
       <c r="H8" s="34" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="I8" s="44" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="38" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B9" s="38" t="s">
         <v>202</v>
@@ -2014,15 +2021,15 @@
       <c r="F9" s="38"/>
       <c r="G9" s="49"/>
       <c r="H9" s="34" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="I9" s="27" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="38" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B10" s="38" t="s">
         <v>91</v>
@@ -2041,10 +2048,10 @@
       </c>
       <c r="G10" s="49"/>
       <c r="H10" s="35" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="I10" s="37" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="87" x14ac:dyDescent="0.35">
@@ -2068,10 +2075,10 @@
       </c>
       <c r="G11" s="49"/>
       <c r="H11" s="35" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="I11" s="37" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -2095,13 +2102,13 @@
       </c>
       <c r="G12" s="49"/>
       <c r="H12" s="35" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="I12" s="37" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="38" t="s">
         <v>217</v>
       </c>
@@ -2116,10 +2123,10 @@
       <c r="F13" s="38"/>
       <c r="G13" s="49"/>
       <c r="H13" s="35" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="I13" s="37" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -2141,7 +2148,7 @@
     </row>
     <row r="15" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="38" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="B15" s="38" t="s">
         <v>203</v>
@@ -2156,15 +2163,15 @@
       <c r="F15" s="38"/>
       <c r="G15" s="49"/>
       <c r="H15" s="34" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="I15" s="27" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="50" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="B16" s="50" t="s">
         <v>204</v>
@@ -2179,10 +2186,10 @@
       <c r="F16" s="38"/>
       <c r="G16" s="49"/>
       <c r="H16" s="34" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="I16" s="27" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -2202,15 +2209,15 @@
       <c r="F17" s="26"/>
       <c r="G17" s="26"/>
       <c r="H17" s="27" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="I17" s="27" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="38" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="B18" s="51" t="s">
         <v>214</v>
@@ -2224,12 +2231,8 @@
       </c>
       <c r="F18" s="26"/>
       <c r="G18" s="26"/>
-      <c r="H18" s="27" t="s">
-        <v>230</v>
-      </c>
-      <c r="I18" s="27" t="s">
-        <v>247</v>
-      </c>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I20" s="52"/>
@@ -2244,12 +2247,88 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBF5162B-B2C4-4F7B-B896-E345E78663FD}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="7" max="7" width="12.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="40" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1" s="40" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1" s="40" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>199</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>200</v>
+      </c>
+      <c r="E2" s="43" t="s">
+        <v>206</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="42" t="s">
+        <v>230</v>
+      </c>
+      <c r="H2" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="I2" s="43" t="s">
+        <v>205</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0A4A292-240A-4D5D-90BA-625919CD3573}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2284,22 +2363,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="26" t="s">
-        <v>111</v>
+        <v>21</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>104</v>
+        <v>136</v>
       </c>
       <c r="D2" s="26" t="s">
         <v>103</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
       <c r="F2" s="26" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -9561,10 +9640,46 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3D8CAB-0E14-4279-809A-3C7733342420}">
+  <dimension ref="M1:N2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="13" max="13" width="17.36328125" customWidth="1"/>
+    <col min="14" max="14" width="16.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="13:14" x14ac:dyDescent="0.35">
+      <c r="M1" s="32" t="s">
+        <v>247</v>
+      </c>
+      <c r="N1" s="32" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="2" spans="13:14" x14ac:dyDescent="0.35">
+      <c r="M2" s="53">
+        <v>87678765</v>
+      </c>
+      <c r="N2" s="53">
+        <v>87688765</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F5E7B35-3B13-4283-A904-8C8CA7625FAB}">
   <dimension ref="A1:AY88"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
+    <sheetView topLeftCell="Y1" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -18998,12 +19113,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F11D5283-EA1B-4FFD-A8B1-716D2E628F52}">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19045,22 +19160,22 @@
         <v>21</v>
       </c>
       <c r="B2" s="40" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C2" s="40" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D2" s="40" t="s">
+        <v>226</v>
+      </c>
+      <c r="E2" s="43" t="s">
         <v>224</v>
-      </c>
-      <c r="E2" s="43" t="s">
-        <v>221</v>
       </c>
       <c r="F2" s="40" t="s">
         <v>20</v>
       </c>
       <c r="G2" s="42" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="H2" s="40" t="s">
         <v>191</v>
@@ -19077,12 +19192,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ACE6922-48CC-4DAE-B734-2DA1995626B5}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19153,80 +19268,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBF5162B-B2C4-4F7B-B896-E345E78663FD}">
-  <dimension ref="A1:I2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8:J9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="7" max="7" width="12.08984375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="40" t="s">
-        <v>185</v>
-      </c>
-      <c r="C1" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="40" t="s">
-        <v>186</v>
-      </c>
-      <c r="E1" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="40" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="40" t="s">
-        <v>187</v>
-      </c>
-      <c r="H1" s="40" t="s">
-        <v>188</v>
-      </c>
-      <c r="I1" s="40" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="40" t="s">
-        <v>199</v>
-      </c>
-      <c r="C2" s="40" t="s">
-        <v>190</v>
-      </c>
-      <c r="D2" s="40" t="s">
-        <v>200</v>
-      </c>
-      <c r="E2" s="43" t="s">
-        <v>206</v>
-      </c>
-      <c r="F2" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="42" t="s">
-        <v>227</v>
-      </c>
-      <c r="H2" s="40" t="s">
-        <v>191</v>
-      </c>
-      <c r="I2" s="43" t="s">
-        <v>205</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Main drop down fixes
Fixes
</commit_message>
<xml_diff>
--- a/ILR_TestSuite/MIP UAT Test Scenarios/TestData.xlsx
+++ b/ILR_TestSuite/MIP UAT Test Scenarios/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\E697642\Documents\GitHub\ILR_TestSuite\ILR_TestSuite\MIP UAT Test Scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G992127\Documents\GitHub\ILR_TestSuite\ILR_TestSuite\MIP UAT Test Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF56E4DC-8504-4B62-BC81-FE22D7D3B86F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A787E33-E315-4BA1-BCBC-A8BAE454D4AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Policy-Servicing" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="198">
   <si>
     <t>Policy No</t>
   </si>
@@ -279,9 +279,6 @@
     <t>IncreaseSumAssured</t>
   </si>
   <si>
-    <t>SS00256539</t>
-  </si>
-  <si>
     <t>Department</t>
   </si>
   <si>
@@ -585,24 +582,64 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Safrican Just Funeral (3000)</t>
-  </si>
-  <si>
-    <t>OpenQA.Selenium.NoSuchElementException: Cannot locate option with value: 110000_x000D_
-   at OpenQA.Selenium.Support.UI.SelectElement.SelectByValue(String value)_x000D_
-   at PolicyServicing.PolicyServicing.IncreaseSumAssured(String contractRef) in C:\Users\E697642\D</t>
-  </si>
-  <si>
     <t>DecreaseSumAssured</t>
   </si>
   <si>
-    <t>Passed</t>
-  </si>
-  <si>
-    <t>19/01/2022 16:22:52</t>
-  </si>
-  <si>
-    <t>19/01/2022 16:24:36</t>
+    <t>Lastname</t>
+  </si>
+  <si>
+    <t>AddRolePlayer</t>
+  </si>
+  <si>
+    <t>TerminateRolePlayer</t>
+  </si>
+  <si>
+    <t>AddRole_NextMonth</t>
+  </si>
+  <si>
+    <t>PostDatedDowngrade</t>
+  </si>
+  <si>
+    <t>PostDatedUpgrade</t>
+  </si>
+  <si>
+    <t>IncreaseSumAssuredAge</t>
+  </si>
+  <si>
+    <t>RemovalOfNonCompulsoryLife</t>
+  </si>
+  <si>
+    <t>ChangeCollectionMeth</t>
+  </si>
+  <si>
+    <t>ReInstate</t>
+  </si>
+  <si>
+    <t>ChangeLifeAssured</t>
+  </si>
+  <si>
+    <t>AddaLife</t>
+  </si>
+  <si>
+    <t>addBeneficiary</t>
+  </si>
+  <si>
+    <t>ChangeCollectionM</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>SS72244130</t>
+  </si>
+  <si>
+    <t>SS03946734</t>
+  </si>
+  <si>
+    <t>CancelPolicy</t>
+  </si>
+  <si>
+    <t>SS11100095</t>
   </si>
 </sst>
 </file>
@@ -612,7 +649,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="###########################0.00#########"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -694,6 +731,13 @@
     <font>
       <sz val="11"/>
       <color theme="9" tint="0.79998168889431442"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF111111"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -814,7 +858,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -862,9 +906,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -905,16 +946,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -931,13 +968,7 @@
     <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -947,19 +978,22 @@
     <xf numFmtId="49" fontId="2" fillId="9" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1395,8 +1429,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{609B3FE1-602A-411C-91B1-C1CE8676CFCE}" name="Table1" displayName="Table1" ref="A1:J14" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10">
-  <autoFilter ref="A1:J14" xr:uid="{609B3FE1-602A-411C-91B1-C1CE8676CFCE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{609B3FE1-602A-411C-91B1-C1CE8676CFCE}" name="Table1" displayName="Table1" ref="A1:J18" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+  <autoFilter ref="A1:J18" xr:uid="{609B3FE1-602A-411C-91B1-C1CE8676CFCE}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{F815EF09-5A8D-41CD-9C8D-1F1F859054C1}" name="Policy No" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{A75649DE-6DED-4E66-9436-0C7BC08EC505}" name="Function" dataDxfId="8"/>
@@ -1709,11 +1743,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{122D3D24-972A-41AA-875A-C35A49A85BBB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{122D3D24-972A-41AA-875A-C35A49A85BBB}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0" rightToLeft="false">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1722,7 +1756,7 @@
     <col min="2" max="2" width="35.1796875" customWidth="1"/>
     <col min="3" max="3" width="43.36328125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.6328125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="16.36328125" customWidth="1"/>
+    <col min="5" max="5" width="24.90625" customWidth="1"/>
     <col min="6" max="6" width="25.1796875" customWidth="1"/>
     <col min="7" max="7" width="17.81640625" customWidth="1"/>
     <col min="8" max="8" width="16.1796875" customWidth="1"/>
@@ -1730,266 +1764,313 @@
     <col min="10" max="10" width="24.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="45" t="s">
+    <row spans="1:10" s="1" customFormat="1" ht="18.5" x14ac:dyDescent="0.45" outlineLevel="0" r="1">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="61" t="s">
+      <c r="I1" s="56" t="s">
+        <v>177</v>
+      </c>
+      <c r="J1" s="44" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="2">
+      <c r="A2" s="37" t="s">
+        <v>197</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="33" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="I2" s="58" t="inlineStr">
+        <is>
+          <t>Object reference not set to an instance of an object</t>
+        </is>
+      </c>
+      <c r="J2" s="52" t="inlineStr">
+        <is>
+          <t>26/01/2022 11:22:54</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="3">
+      <c r="A3" s="64" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37" t="inlineStr">
+        <is>
+          <t>Safrican Just Funeral (3000)</t>
+        </is>
+      </c>
+      <c r="F3" s="37"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="34" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="I3" s="59" t="inlineStr">
+        <is>
+          <t>no such element: Unable to locate element: method:css selectorselector:*[name=fcCollectionMethod]
+  (Session info: chrome=9604664110)</t>
+        </is>
+      </c>
+      <c r="J3" s="53" t="inlineStr">
+        <is>
+          <t>26/01/2022 11:26:52</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="4">
+      <c r="A4" s="64" t="s">
+        <v>195</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37" t="inlineStr">
+        <is>
+          <t>Safrican Just Funeral (3000)</t>
+        </is>
+      </c>
+      <c r="F4" s="37"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="33" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="I4" s="57"/>
+      <c r="J4" s="52" t="inlineStr">
+        <is>
+          <t>26/01/2022 11:30:38</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="5">
+      <c r="A5" s="64" t="s">
+        <v>195</v>
+      </c>
+      <c r="B5" s="37" t="s">
         <v>178</v>
       </c>
-      <c r="J1" s="45" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="123" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="B2" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="68" t="s">
-        <v>179</v>
-      </c>
-      <c r="F2" s="38"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="34" t="s">
-        <v>182</v>
-      </c>
-      <c r="I2" s="62" t="s">
-        <v>180</v>
-      </c>
-      <c r="J2" s="27" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="54" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="38" t="s">
-        <v>181</v>
-      </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="68" t="s">
-        <v>179</v>
-      </c>
-      <c r="F3" s="38"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="34" t="s">
-        <v>182</v>
-      </c>
-      <c r="I3" s="63"/>
-      <c r="J3" s="55" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="54"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="56"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="38"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="27"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="38"/>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="49"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37" t="inlineStr">
+        <is>
+          <t>Safrican Just Funeral (3000)</t>
+        </is>
+      </c>
+      <c r="F5" s="37"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="33" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="I5" s="57"/>
+      <c r="J5" s="52" t="inlineStr">
+        <is>
+          <t>26/01/2022 11:34:36</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="6">
+      <c r="A6" s="51"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="47"/>
       <c r="H6" s="34"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="27"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="38"/>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="65"/>
-      <c r="J7" s="36"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="38"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="62"/>
-      <c r="J8" s="44"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="38"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="62"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="53"/>
+    </row>
+    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="7">
+      <c r="A7" s="37"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="35"/>
+    </row>
+    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="8">
+      <c r="A8" s="37"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="43"/>
+    </row>
+    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="9">
+      <c r="A9" s="37"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="57"/>
       <c r="J9" s="27"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="38"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="65"/>
-      <c r="J10" s="37"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="39"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="65"/>
-      <c r="J11" s="37"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="38"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="65"/>
-      <c r="J12" s="37"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="38"/>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="65"/>
-      <c r="J13" s="37"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="38"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="65"/>
-      <c r="J14" s="37"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="38"/>
-      <c r="B15" s="38"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="62"/>
-      <c r="J15" s="27"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="50"/>
-      <c r="B16" s="50"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="58"/>
-      <c r="G16" s="59"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="66"/>
-      <c r="J16" s="60"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="38"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="67"/>
-      <c r="J17" s="27"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="50"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="67"/>
-      <c r="J18" s="27"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="J20" s="52"/>
+    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="10">
+      <c r="A10" s="37"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="36"/>
+    </row>
+    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="11">
+      <c r="A11" s="38"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="36"/>
+    </row>
+    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="12">
+      <c r="A12" s="37"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="59"/>
+      <c r="J12" s="36"/>
+    </row>
+    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="13">
+      <c r="A13" s="37"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="59"/>
+      <c r="J13" s="36"/>
+    </row>
+    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="14">
+      <c r="A14" s="37"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="59"/>
+      <c r="J14" s="36"/>
+    </row>
+    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="15">
+      <c r="A15" s="51"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="52"/>
+    </row>
+    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="16">
+      <c r="A16" s="62"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="55"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="57"/>
+      <c r="J16" s="52"/>
+    </row>
+    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="17">
+      <c r="A17" s="51"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="57"/>
+      <c r="J17" s="52"/>
+    </row>
+    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="18">
+      <c r="A18" s="62"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="52"/>
+    </row>
+    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="20">
+      <c r="J20" s="49"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1998,6 +2079,18 @@
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6B7A0E4F-DDE3-4826-92F4-603E836DB70E}">
+          <x14:formula1>
+            <xm:f>Dropdown!$G$2:$G$17</xm:f>
+          </x14:formula1>
+          <xm:sqref>B7:B18 B2:B5</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2015,61 +2108,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="39" t="s">
         <v>150</v>
       </c>
-      <c r="C1" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="40" t="s">
+      <c r="E1" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="E1" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="40" t="s">
+      <c r="H1" s="39" t="s">
         <v>152</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="I1" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="I1" s="40" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" s="39" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="40" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="40" t="s">
+      <c r="D2" s="39" t="s">
         <v>164</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="E2" s="42" t="s">
+        <v>166</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="H2" s="39" t="s">
         <v>155</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="I2" s="42" t="s">
         <v>165</v>
-      </c>
-      <c r="E2" s="43" t="s">
-        <v>167</v>
-      </c>
-      <c r="F2" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="42" t="s">
-        <v>175</v>
-      </c>
-      <c r="H2" s="40" t="s">
-        <v>156</v>
-      </c>
-      <c r="I2" s="43" t="s">
-        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2103,16 +2196,16 @@
         <v>11</v>
       </c>
       <c r="C1" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="32" t="s">
         <v>80</v>
-      </c>
-      <c r="D1" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="E1" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="F1" s="32" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -2120,19 +2213,19 @@
         <v>18</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F2" s="26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2143,37 +2236,37 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D789A2EE-1FAB-4DF2-80EC-2E2D01AB4288}">
           <x14:formula1>
-            <xm:f>Dropdown!$A$1:$A$12</xm:f>
+            <xm:f>Dropdown!$A$2:$A$13</xm:f>
           </x14:formula1>
           <xm:sqref>E2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BD36C127-308E-4832-B090-AE5EB6F016EB}">
           <x14:formula1>
-            <xm:f>Dropdown!$B$1:$B$19</xm:f>
+            <xm:f>Dropdown!$B$2:$B$20</xm:f>
           </x14:formula1>
           <xm:sqref>A2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0A704850-6031-4011-B17B-96DE3135B4BD}">
           <x14:formula1>
-            <xm:f>Dropdown!$C$1:$C$10</xm:f>
+            <xm:f>Dropdown!$C$2:$C$11</xm:f>
           </x14:formula1>
           <xm:sqref>B2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D07E571C-59CE-47F3-B108-2A4C3E71F699}">
           <x14:formula1>
-            <xm:f>Dropdown!$D$1:$D$8</xm:f>
+            <xm:f>Dropdown!$D$2:$D$9</xm:f>
           </x14:formula1>
           <xm:sqref>C2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4D86FE76-8C47-4433-B99D-5E721117AB72}">
           <x14:formula1>
-            <xm:f>Dropdown!$E$1:$E$6</xm:f>
+            <xm:f>Dropdown!$E$2:$E$7</xm:f>
           </x14:formula1>
           <xm:sqref>D2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{86F0C28B-0B2D-4E3F-82F7-144F83220CE5}">
           <x14:formula1>
-            <xm:f>Dropdown!$F$1:$F$19</xm:f>
+            <xm:f>Dropdown!$F$2:$F$20</xm:f>
           </x14:formula1>
           <xm:sqref>F2</xm:sqref>
         </x14:dataValidation>
@@ -9041,9 +9134,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0280A1E1-10C8-479A-A428-3162F59DEFE5}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -9052,271 +9147,332 @@
     <col min="3" max="3" width="27.1796875" customWidth="1"/>
     <col min="4" max="4" width="34.54296875" customWidth="1"/>
     <col min="5" max="5" width="29.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="56.90625" style="61" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>163</v>
-      </c>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E1" t="s">
-        <v>119</v>
-      </c>
-      <c r="F1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+        <v>179</v>
+      </c>
+      <c r="G1" s="63" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>162</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D2" t="s">
         <v>112</v>
       </c>
       <c r="E2" t="s">
-        <v>83</v>
+        <v>118</v>
       </c>
       <c r="F2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>123</v>
+      </c>
+      <c r="G2" s="50" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>161</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E3" t="s">
-        <v>120</v>
+        <v>82</v>
       </c>
       <c r="F3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>124</v>
+      </c>
+      <c r="G3" s="50" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>160</v>
       </c>
       <c r="B4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G4" s="50" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" t="s">
+        <v>120</v>
+      </c>
+      <c r="F5" t="s">
+        <v>126</v>
+      </c>
+      <c r="G5" s="50" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B6" t="s">
         <v>87</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C6" t="s">
         <v>106</v>
       </c>
-      <c r="D4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E6" t="s">
         <v>121</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F6" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="G6" s="50" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>158</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>88</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G7" s="50" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" t="s">
         <v>107</v>
       </c>
-      <c r="D5" t="s">
-        <v>115</v>
-      </c>
-      <c r="E5" t="s">
-        <v>122</v>
-      </c>
-      <c r="F5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>159</v>
-      </c>
-      <c r="B6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="D8" t="s">
         <v>116</v>
       </c>
-      <c r="E6" t="s">
-        <v>123</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="F8" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="G8" s="50" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C9" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" t="s">
+        <v>117</v>
+      </c>
+      <c r="F9" t="s">
+        <v>130</v>
+      </c>
+      <c r="G9" s="50" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>144</v>
+      </c>
+      <c r="B10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" t="s">
+        <v>109</v>
+      </c>
+      <c r="F10" t="s">
+        <v>131</v>
+      </c>
+      <c r="G10" s="50" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>142</v>
       </c>
-      <c r="B7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C7" t="s">
-        <v>108</v>
-      </c>
-      <c r="D7" t="s">
-        <v>117</v>
-      </c>
-      <c r="F7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>144</v>
-      </c>
-      <c r="B8" t="s">
-        <v>148</v>
-      </c>
-      <c r="C8" t="s">
-        <v>109</v>
-      </c>
-      <c r="D8" t="s">
-        <v>118</v>
-      </c>
-      <c r="F8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="B11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" t="s">
+        <v>110</v>
+      </c>
+      <c r="F11" t="s">
+        <v>132</v>
+      </c>
+      <c r="G11" s="50" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>145</v>
       </c>
-      <c r="B9" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" t="s">
-        <v>110</v>
-      </c>
-      <c r="F9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>143</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>92</v>
       </c>
-      <c r="C10" t="s">
-        <v>111</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="F12" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="G12" s="50" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>146</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" t="s">
         <v>93</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F13" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>147</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="G13" s="50" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
         <v>94</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F14" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" s="50" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>95</v>
+      </c>
+      <c r="F15" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
-        <v>95</v>
-      </c>
-      <c r="F13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
+      <c r="G15" s="50" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
         <v>96</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F16" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B15" t="s">
+      <c r="G16" s="50" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
         <v>97</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F17" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B16" t="s">
+      <c r="G17" s="50" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
         <v>98</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F18" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B17" t="s">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
         <v>99</v>
-      </c>
-      <c r="F17" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B18" t="s">
-        <v>100</v>
-      </c>
-      <c r="F18" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B19" t="s">
-        <v>101</v>
       </c>
       <c r="F19" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>149</v>
+        <v>100</v>
+      </c>
+      <c r="F20" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -9409,17 +9565,17 @@
   <sheetData>
     <row r="1" spans="13:14" x14ac:dyDescent="0.35">
       <c r="M1" s="32" t="s">
+        <v>175</v>
+      </c>
+      <c r="N1" s="32" t="s">
         <v>176</v>
       </c>
-      <c r="N1" s="32" t="s">
-        <v>177</v>
-      </c>
     </row>
     <row r="2" spans="13:14" x14ac:dyDescent="0.35">
-      <c r="M2" s="53">
+      <c r="M2" s="50">
         <v>87678765</v>
       </c>
-      <c r="N2" s="53">
+      <c r="N2" s="50">
         <v>87688765</v>
       </c>
     </row>
@@ -18881,60 +19037,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="39" t="s">
         <v>150</v>
       </c>
-      <c r="C1" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="40" t="s">
+      <c r="E1" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="F1" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="E1" s="40" t="s">
-        <v>157</v>
-      </c>
-      <c r="F1" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="40" t="s">
+      <c r="H1" s="39" t="s">
         <v>152</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="I1" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="I1" s="40" t="s">
-        <v>154</v>
-      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="39" t="s">
+        <v>171</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="D2" s="39" t="s">
         <v>172</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="E2" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="41" t="s">
         <v>169</v>
       </c>
-      <c r="D2" s="40" t="s">
-        <v>173</v>
-      </c>
-      <c r="E2" s="43" t="s">
-        <v>171</v>
-      </c>
-      <c r="F2" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="42" t="s">
-        <v>170</v>
-      </c>
-      <c r="H2" s="40" t="s">
-        <v>156</v>
-      </c>
-      <c r="I2" s="41">
+      <c r="H2" s="39" t="s">
+        <v>155</v>
+      </c>
+      <c r="I2" s="40">
         <v>44562</v>
       </c>
     </row>
@@ -18961,61 +19117,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="39" t="s">
         <v>150</v>
       </c>
-      <c r="C1" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="40" t="s">
+      <c r="E1" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="E1" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="40" t="s">
+      <c r="H1" s="39" t="s">
         <v>152</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="I1" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="I1" s="40" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" s="39" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="40" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="40" t="s">
+      <c r="D2" s="39" t="s">
         <v>164</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="E2" s="42" t="s">
+        <v>166</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="41" t="s">
+        <v>173</v>
+      </c>
+      <c r="H2" s="39" t="s">
         <v>155</v>
       </c>
-      <c r="D2" s="40" t="s">
-        <v>165</v>
-      </c>
-      <c r="E2" s="43" t="s">
+      <c r="I2" s="42" t="s">
         <v>167</v>
-      </c>
-      <c r="F2" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="42" t="s">
-        <v>174</v>
-      </c>
-      <c r="H2" s="40" t="s">
-        <v>156</v>
-      </c>
-      <c r="I2" s="43" t="s">
-        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reinstate fix and collection method fix
</commit_message>
<xml_diff>
--- a/ILR_TestSuite/MIP UAT Test Scenarios/TestData.xlsx
+++ b/ILR_TestSuite/MIP UAT Test Scenarios/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G992127\Documents\GitHub\ILR_TestSuite\ILR_TestSuite\MIP UAT Test Scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G992107\Documents\GitHub\ILR_TestSuite\ILR_TestSuite\MIP UAT Test Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A787E33-E315-4BA1-BCBC-A8BAE454D4AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E615A7-5240-4C6B-BAC1-42CC95C540B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2400" yWindow="1720" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Policy-Servicing" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="207">
   <si>
     <t>Policy No</t>
   </si>
@@ -630,16 +630,44 @@
     <t>Method</t>
   </si>
   <si>
-    <t>SS72244130</t>
-  </si>
-  <si>
-    <t>SS03946734</t>
-  </si>
-  <si>
     <t>CancelPolicy</t>
   </si>
   <si>
-    <t>SS11100095</t>
+    <t>SS03946733</t>
+  </si>
+  <si>
+    <t>SK88115509</t>
+  </si>
+  <si>
+    <t>SS00946925</t>
+  </si>
+  <si>
+    <t>Safrican Serenity Funeral Premium (1000)</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>26/01/2022 14:52:51</t>
+  </si>
+  <si>
+    <t>Safrican Just Funeral (3000)</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>26/01/2022 14:54:23</t>
+  </si>
+  <si>
+    <t>element not interactable
+  (Session info: chrome=9604664110)</t>
+  </si>
+  <si>
+    <t>26/01/2022 14:55:16</t>
+  </si>
+  <si>
+    <t>26/01/2022 14:56:40</t>
   </si>
 </sst>
 </file>
@@ -649,7 +677,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="###########################0.00#########"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -741,6 +769,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF111111"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="11">
@@ -912,9 +947,6 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -935,9 +967,6 @@
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -996,6 +1025,8 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1429,8 +1460,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{609B3FE1-602A-411C-91B1-C1CE8676CFCE}" name="Table1" displayName="Table1" ref="A1:J18" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10">
-  <autoFilter ref="A1:J18" xr:uid="{609B3FE1-602A-411C-91B1-C1CE8676CFCE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{609B3FE1-602A-411C-91B1-C1CE8676CFCE}" name="Table1" displayName="Table1" ref="A1:J14" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+  <autoFilter ref="A1:J14" xr:uid="{609B3FE1-602A-411C-91B1-C1CE8676CFCE}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{F815EF09-5A8D-41CD-9C8D-1F1F859054C1}" name="Policy No" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{A75649DE-6DED-4E66-9436-0C7BC08EC505}" name="Function" dataDxfId="8"/>
@@ -1743,11 +1774,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{122D3D24-972A-41AA-875A-C35A49A85BBB}">
-  <dimension ref="A1:J20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{122D3D24-972A-41AA-875A-C35A49A85BBB}">
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1764,313 +1795,238 @@
     <col min="10" max="10" width="24.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row spans="1:10" s="1" customFormat="1" ht="18.5" x14ac:dyDescent="0.45" outlineLevel="0" r="1">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="44" t="s">
+      <c r="G1" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="44" t="s">
+      <c r="H1" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="56" t="s">
+      <c r="I1" s="54" t="s">
         <v>177</v>
       </c>
-      <c r="J1" s="44" t="s">
+      <c r="J1" s="42" t="s">
         <v>8</v>
       </c>
     </row>
-    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="2">
-      <c r="A2" s="37" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="63" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="58" t="s">
+        <v>198</v>
+      </c>
+      <c r="F2" s="36"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="33" t="s">
+        <v>199</v>
+      </c>
+      <c r="I2" s="56"/>
+      <c r="J2" s="50" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="62" t="s">
         <v>197</v>
       </c>
-      <c r="B2" s="37" t="s">
-        <v>188</v>
-      </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="33" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-      <c r="I2" s="58" t="inlineStr">
-        <is>
-          <t>Object reference not set to an instance of an object</t>
-        </is>
-      </c>
-      <c r="J2" s="52" t="inlineStr">
-        <is>
-          <t>26/01/2022 11:22:54</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="3">
-      <c r="A3" s="64" t="s">
-        <v>194</v>
-      </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="36" t="s">
         <v>192</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37" t="inlineStr">
-        <is>
-          <t>Safrican Just Funeral (3000)</t>
-        </is>
-      </c>
-      <c r="F3" s="37"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="34" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-      <c r="I3" s="59" t="inlineStr">
-        <is>
-          <t>no such element: Unable to locate element: method:css selectorselector:*[name=fcCollectionMethod]
-  (Session info: chrome=9604664110)</t>
-        </is>
-      </c>
-      <c r="J3" s="53" t="inlineStr">
-        <is>
-          <t>26/01/2022 11:26:52</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="4">
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36" t="s">
+        <v>201</v>
+      </c>
+      <c r="F3" s="36"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="I3" s="57"/>
+      <c r="J3" s="51" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="64" t="s">
+        <v>197</v>
+      </c>
+      <c r="B4" s="36" t="s">
+        <v>187</v>
+      </c>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36" t="s">
+        <v>201</v>
+      </c>
+      <c r="F4" s="36"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="I4" s="57" t="s">
+        <v>204</v>
+      </c>
+      <c r="J4" s="51" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="36" t="s">
         <v>195</v>
       </c>
-      <c r="B4" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37" t="inlineStr">
-        <is>
-          <t>Safrican Just Funeral (3000)</t>
-        </is>
-      </c>
-      <c r="F4" s="37"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="33" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="I4" s="57"/>
-      <c r="J4" s="52" t="inlineStr">
-        <is>
-          <t>26/01/2022 11:30:38</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="5">
-      <c r="A5" s="64" t="s">
-        <v>195</v>
-      </c>
-      <c r="B5" s="37" t="s">
-        <v>178</v>
-      </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37" t="inlineStr">
-        <is>
-          <t>Safrican Just Funeral (3000)</t>
-        </is>
-      </c>
-      <c r="F5" s="37"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="33" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="I5" s="57"/>
-      <c r="J5" s="52" t="inlineStr">
-        <is>
-          <t>26/01/2022 11:34:36</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="6">
-      <c r="A6" s="51"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="47"/>
+      <c r="B5" s="36" t="s">
+        <v>185</v>
+      </c>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36" t="s">
+        <v>201</v>
+      </c>
+      <c r="F5" s="36"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="33" t="s">
+        <v>202</v>
+      </c>
+      <c r="I5" s="55"/>
+      <c r="J5" s="27" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="36"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="45"/>
       <c r="H6" s="34"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="53"/>
-    </row>
-    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="7">
+      <c r="I6" s="57"/>
+      <c r="J6" s="35"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="37"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="47"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="45"/>
       <c r="H7" s="34"/>
-      <c r="I7" s="59"/>
+      <c r="I7" s="57"/>
       <c r="J7" s="35"/>
     </row>
-    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="8">
-      <c r="A8" s="37"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="33"/>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="36"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="34"/>
       <c r="I8" s="57"/>
-      <c r="J8" s="43"/>
-    </row>
-    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="9">
-      <c r="A9" s="37"/>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="33"/>
+      <c r="J8" s="35"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="36"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="34"/>
       <c r="I9" s="57"/>
-      <c r="J9" s="27"/>
-    </row>
-    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="10">
-      <c r="A10" s="37"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="47"/>
+      <c r="J9" s="35"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="36"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="45"/>
       <c r="H10" s="34"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="36"/>
-    </row>
-    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="11">
-      <c r="A11" s="38"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="59"/>
-      <c r="J11" s="36"/>
-    </row>
-    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="12">
-      <c r="A12" s="37"/>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="59"/>
-      <c r="J12" s="36"/>
-    </row>
-    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="13">
-      <c r="A13" s="37"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="36"/>
-    </row>
-    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="14">
-      <c r="A14" s="37"/>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="59"/>
-      <c r="J14" s="36"/>
-    </row>
-    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="15">
-      <c r="A15" s="51"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="57"/>
-      <c r="J15" s="52"/>
-    </row>
-    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="16">
-      <c r="A16" s="62"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="57"/>
-      <c r="J16" s="52"/>
-    </row>
-    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="17">
-      <c r="A17" s="51"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="57"/>
-      <c r="J17" s="52"/>
-    </row>
-    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="18">
-      <c r="A18" s="62"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="57"/>
-      <c r="J18" s="52"/>
-    </row>
-    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="20">
-      <c r="J20" s="49"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="35"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="49"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="50"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="60"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="50"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="49"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="50"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="60"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="55"/>
+      <c r="J14" s="50"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J16" s="47"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -2086,7 +2042,7 @@
           <x14:formula1>
             <xm:f>Dropdown!$G$2:$G$17</xm:f>
           </x14:formula1>
-          <xm:sqref>B7:B18 B2:B5</xm:sqref>
+          <xm:sqref>B2:B14</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2108,60 +2064,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="38" t="s">
         <v>151</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="38" t="s">
         <v>152</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="I1" s="38" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="38" t="s">
         <v>163</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="38" t="s">
         <v>164</v>
       </c>
-      <c r="E2" s="42" t="s">
+      <c r="E2" s="41" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="40" t="s">
         <v>174</v>
       </c>
-      <c r="H2" s="39" t="s">
+      <c r="H2" s="38" t="s">
         <v>155</v>
       </c>
-      <c r="I2" s="42" t="s">
+      <c r="I2" s="41" t="s">
         <v>165</v>
       </c>
     </row>
@@ -9148,7 +9104,7 @@
     <col min="4" max="4" width="34.54296875" customWidth="1"/>
     <col min="5" max="5" width="29.36328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="56.90625" style="61" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="56.90625" style="59" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -9158,7 +9114,7 @@
       <c r="C1" t="s">
         <v>179</v>
       </c>
-      <c r="G1" s="63" t="s">
+      <c r="G1" s="61" t="s">
         <v>193</v>
       </c>
     </row>
@@ -9181,7 +9137,7 @@
       <c r="F2" t="s">
         <v>123</v>
       </c>
-      <c r="G2" s="50" t="s">
+      <c r="G2" s="48" t="s">
         <v>180</v>
       </c>
     </row>
@@ -9204,7 +9160,7 @@
       <c r="F3" t="s">
         <v>124</v>
       </c>
-      <c r="G3" s="50" t="s">
+      <c r="G3" s="48" t="s">
         <v>181</v>
       </c>
     </row>
@@ -9227,7 +9183,7 @@
       <c r="F4" t="s">
         <v>125</v>
       </c>
-      <c r="G4" s="50" t="s">
+      <c r="G4" s="48" t="s">
         <v>76</v>
       </c>
     </row>
@@ -9250,7 +9206,7 @@
       <c r="F5" t="s">
         <v>126</v>
       </c>
-      <c r="G5" s="50" t="s">
+      <c r="G5" s="48" t="s">
         <v>178</v>
       </c>
     </row>
@@ -9273,7 +9229,7 @@
       <c r="F6" t="s">
         <v>127</v>
       </c>
-      <c r="G6" s="50" t="s">
+      <c r="G6" s="48" t="s">
         <v>182</v>
       </c>
     </row>
@@ -9296,7 +9252,7 @@
       <c r="F7" t="s">
         <v>128</v>
       </c>
-      <c r="G7" s="50" t="s">
+      <c r="G7" s="48" t="s">
         <v>183</v>
       </c>
     </row>
@@ -9316,7 +9272,7 @@
       <c r="F8" t="s">
         <v>129</v>
       </c>
-      <c r="G8" s="50" t="s">
+      <c r="G8" s="48" t="s">
         <v>184</v>
       </c>
     </row>
@@ -9336,7 +9292,7 @@
       <c r="F9" t="s">
         <v>130</v>
       </c>
-      <c r="G9" s="50" t="s">
+      <c r="G9" s="48" t="s">
         <v>185</v>
       </c>
     </row>
@@ -9353,7 +9309,7 @@
       <c r="F10" t="s">
         <v>131</v>
       </c>
-      <c r="G10" s="50" t="s">
+      <c r="G10" s="48" t="s">
         <v>186</v>
       </c>
     </row>
@@ -9370,7 +9326,7 @@
       <c r="F11" t="s">
         <v>132</v>
       </c>
-      <c r="G11" s="50" t="s">
+      <c r="G11" s="48" t="s">
         <v>187</v>
       </c>
     </row>
@@ -9384,7 +9340,7 @@
       <c r="F12" t="s">
         <v>133</v>
       </c>
-      <c r="G12" s="50" t="s">
+      <c r="G12" s="48" t="s">
         <v>188</v>
       </c>
     </row>
@@ -9398,8 +9354,8 @@
       <c r="F13" t="s">
         <v>134</v>
       </c>
-      <c r="G13" s="50" t="s">
-        <v>196</v>
+      <c r="G13" s="48" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -9409,7 +9365,7 @@
       <c r="F14" t="s">
         <v>81</v>
       </c>
-      <c r="G14" s="50" t="s">
+      <c r="G14" s="48" t="s">
         <v>189</v>
       </c>
     </row>
@@ -9420,7 +9376,7 @@
       <c r="F15" t="s">
         <v>135</v>
       </c>
-      <c r="G15" s="50" t="s">
+      <c r="G15" s="48" t="s">
         <v>190</v>
       </c>
     </row>
@@ -9431,7 +9387,7 @@
       <c r="F16" t="s">
         <v>136</v>
       </c>
-      <c r="G16" s="50" t="s">
+      <c r="G16" s="48" t="s">
         <v>191</v>
       </c>
     </row>
@@ -9442,7 +9398,7 @@
       <c r="F17" t="s">
         <v>137</v>
       </c>
-      <c r="G17" s="50" t="s">
+      <c r="G17" s="48" t="s">
         <v>192</v>
       </c>
     </row>
@@ -9554,7 +9510,7 @@
   <dimension ref="M1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9572,11 +9528,11 @@
       </c>
     </row>
     <row r="2" spans="13:14" x14ac:dyDescent="0.35">
-      <c r="M2" s="50">
-        <v>87678765</v>
-      </c>
-      <c r="N2" s="50">
-        <v>87688765</v>
+      <c r="M2" s="48">
+        <v>87678265</v>
+      </c>
+      <c r="N2" s="48">
+        <v>98778678</v>
       </c>
     </row>
   </sheetData>
@@ -19037,60 +18993,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="38" t="s">
         <v>156</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="38" t="s">
         <v>151</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="38" t="s">
         <v>152</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="I1" s="38" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="E2" s="42" t="s">
+      <c r="E2" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="40" t="s">
         <v>169</v>
       </c>
-      <c r="H2" s="39" t="s">
+      <c r="H2" s="38" t="s">
         <v>155</v>
       </c>
-      <c r="I2" s="40">
+      <c r="I2" s="39">
         <v>44562</v>
       </c>
     </row>
@@ -19117,60 +19073,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="38" t="s">
         <v>151</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="38" t="s">
         <v>152</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="I1" s="38" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="38" t="s">
         <v>163</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="38" t="s">
         <v>164</v>
       </c>
-      <c r="E2" s="42" t="s">
+      <c r="E2" s="41" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="40" t="s">
         <v>173</v>
       </c>
-      <c r="H2" s="39" t="s">
+      <c r="H2" s="38" t="s">
         <v>155</v>
       </c>
-      <c r="I2" s="42" t="s">
+      <c r="I2" s="41" t="s">
         <v>167</v>
       </c>
     </row>

</xml_diff>

<commit_message>
report first draft excel
</commit_message>
<xml_diff>
--- a/ILR_TestSuite/MIP UAT Test Scenarios/TestData.xlsx
+++ b/ILR_TestSuite/MIP UAT Test Scenarios/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\E697642\Documents\GitHub\ILR_TestSuite\ILR_TestSuite\MIP UAT Test Scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G992107\Documents\GitHub\ILR_TestSuite\ILR_TestSuite\MIP UAT Test Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C806651-E3D7-429E-84E4-D5CF72E50B4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E0B5B62-8DE3-445B-9ECD-C3B71176C76D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Policy-Servicing" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="331">
   <si>
     <t>Policy No</t>
   </si>
@@ -977,6 +977,103 @@
   <si>
     <t xml:space="preserve">SS01008981
 </t>
+  </si>
+  <si>
+    <t>Safrican Just Funeral (3000)</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>21/02/2022 10:35:27</t>
+  </si>
+  <si>
+    <t>21/02/2022 10:36:47</t>
+  </si>
+  <si>
+    <t>21/02/2022 10:38:28</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Safrican Just Funeral [3000] is not a valid name Make sure that it does not include invalid characters or punctuation and that it is not too long</t>
+  </si>
+  <si>
+    <t>21/02/2022 10:40:05</t>
+  </si>
+  <si>
+    <t>21/02/2022 10:41:37</t>
+  </si>
+  <si>
+    <t>Safrican Provide and Protect Plan (4000)</t>
+  </si>
+  <si>
+    <t>unexpected alert open: Alert text : There has been an error submitting your page
+Ensure that you have:
+  - Specified all mandatory fields
+  - Specified all fields using the correct format
+Hover over the highlighted controls for a description of the e</t>
+  </si>
+  <si>
+    <t>21/02/2022 10:42:56</t>
+  </si>
+  <si>
+    <t>21/02/2022 10:44:25</t>
+  </si>
+  <si>
+    <t>21/02/2022 10:46:29</t>
+  </si>
+  <si>
+    <t>21/02/2022 10:48:41</t>
+  </si>
+  <si>
+    <t>21/02/2022 10:49:40</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: method:xpathselector://*[id=CntContentsDiv9]/table/tbody/tr[2]/td[4]
+  (Session info: chrome=970469271)</t>
+  </si>
+  <si>
+    <t>21/02/2022 10:51:14</t>
+  </si>
+  <si>
+    <t>21/02/2022 10:52:47</t>
+  </si>
+  <si>
+    <t>21/02/2022 10:54:22</t>
+  </si>
+  <si>
+    <t>Safrican Serenity Funeral Premium (1000)</t>
+  </si>
+  <si>
+    <t>unexpected alert open: Alert text : The same policy payer was found with another employee number Would you like to update the employee number?
+  (Session info: chrome=970469271)</t>
+  </si>
+  <si>
+    <t>21/02/2022 10:55:43</t>
+  </si>
+  <si>
+    <t>String lengths are both 72 Strings differ at index 11_x000D_
+  Expected: tstsafricancoza/web/wspd_cgish/WService=wsb_ilrtst/runw?_x000D_
+  But was:  intsafricancoza/web/wspd_cgish/WService=wsb_ilrint/runw?_x000D_
+  --------------^_x000D_</t>
+  </si>
+  <si>
+    <t>21/02/2022 10:56:41</t>
+  </si>
+  <si>
+    <t>Safrican Serenity Funeral (2000)</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: method:css selectorselector:#t0_749
+  (Session info: chrome=970469271)</t>
+  </si>
+  <si>
+    <t>21/02/2022 10:58:04</t>
+  </si>
+  <si>
+    <t>21/02/2022 10:59:36</t>
   </si>
 </sst>
 </file>
@@ -1017,6 +1114,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2119,10 +2217,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{122D3D24-972A-41AA-875A-C35A49A85BBB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{122D3D24-972A-41AA-875A-C35A49A85BBB}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0" rightToLeft="false">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -2140,7 +2238,7 @@
     <col min="10" max="10" width="24.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row spans="1:10" s="1" customFormat="1" ht="18.5" x14ac:dyDescent="0.45" outlineLevel="0" r="1">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
@@ -2172,7 +2270,7 @@
         <v>8</v>
       </c>
     </row>
-    <row spans="1:10" ht="29" x14ac:dyDescent="0.35" outlineLevel="0" r="2">
+    <row r="2" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="37" t="s">
         <v>280</v>
       </c>
@@ -2183,28 +2281,22 @@
         <v>190</v>
       </c>
       <c r="D2" s="37"/>
-      <c r="E2" s="37" t="inlineStr">
-        <is>
-          <t>Safrican Just Funeral (3000)</t>
-        </is>
+      <c r="E2" s="37" t="s">
+        <v>302</v>
       </c>
       <c r="F2" s="37" t="s">
         <v>207</v>
       </c>
       <c r="G2" s="46"/>
-      <c r="H2" s="33" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
+      <c r="H2" s="33" t="s">
+        <v>303</v>
       </c>
       <c r="I2" s="53"/>
-      <c r="J2" s="49" t="inlineStr">
-        <is>
-          <t>21/02/2022 10:35:27</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="3">
+      <c r="J2" s="49" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="37" t="s">
         <v>280</v>
       </c>
@@ -2215,28 +2307,22 @@
         <v>191</v>
       </c>
       <c r="D3" s="37"/>
-      <c r="E3" s="37" t="inlineStr">
-        <is>
-          <t>Safrican Just Funeral (3000)</t>
-        </is>
+      <c r="E3" s="37" t="s">
+        <v>302</v>
       </c>
       <c r="F3" s="37" t="s">
         <v>207</v>
       </c>
       <c r="G3" s="46"/>
-      <c r="H3" s="33" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
+      <c r="H3" s="33" t="s">
+        <v>303</v>
       </c>
       <c r="I3" s="53"/>
-      <c r="J3" s="49" t="inlineStr">
-        <is>
-          <t>21/02/2022 10:36:47</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:10" ht="29" x14ac:dyDescent="0.35" outlineLevel="0" r="4">
+      <c r="J3" s="49" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="37" t="s">
         <v>285</v>
       </c>
@@ -2247,28 +2333,22 @@
         <v>192</v>
       </c>
       <c r="D4" s="37"/>
-      <c r="E4" s="37" t="inlineStr">
-        <is>
-          <t>Safrican Just Funeral (3000)</t>
-        </is>
+      <c r="E4" s="37" t="s">
+        <v>302</v>
       </c>
       <c r="F4" s="37" t="s">
         <v>207</v>
       </c>
       <c r="G4" s="46"/>
-      <c r="H4" s="34" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
+      <c r="H4" s="34" t="s">
+        <v>303</v>
       </c>
       <c r="I4" s="54"/>
-      <c r="J4" s="50" t="inlineStr">
-        <is>
-          <t>21/02/2022 10:38:28</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:10" ht="58" x14ac:dyDescent="0.35" outlineLevel="0" r="5">
+      <c r="J4" s="50" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="57" t="s">
         <v>280</v>
       </c>
@@ -2279,32 +2359,24 @@
         <v>193</v>
       </c>
       <c r="D5" s="37"/>
-      <c r="E5" s="37" t="inlineStr">
-        <is>
-          <t>Safrican Just Funeral (3000)</t>
-        </is>
+      <c r="E5" s="37" t="s">
+        <v>302</v>
       </c>
       <c r="F5" s="37" t="s">
         <v>207</v>
       </c>
       <c r="G5" s="46"/>
-      <c r="H5" s="34" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-      <c r="I5" s="54" t="inlineStr">
-        <is>
-          <t>Safrican Just Funeral [3000] is not a valid name Make sure that it does not include invalid characters or punctuation and that it is not too long</t>
-        </is>
-      </c>
-      <c r="J5" s="50" t="inlineStr">
-        <is>
-          <t>21/02/2022 10:40:05</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.35" outlineLevel="0" r="6">
+      <c r="H5" s="34" t="s">
+        <v>307</v>
+      </c>
+      <c r="I5" s="54" t="s">
+        <v>308</v>
+      </c>
+      <c r="J5" s="50" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="37" t="s">
         <v>281</v>
       </c>
@@ -2315,32 +2387,24 @@
         <v>194</v>
       </c>
       <c r="D6" s="37"/>
-      <c r="E6" s="37" t="inlineStr">
-        <is>
-          <t>Safrican Just Funeral (3000)</t>
-        </is>
+      <c r="E6" s="37" t="s">
+        <v>302</v>
       </c>
       <c r="F6" s="37" t="s">
         <v>207</v>
       </c>
       <c r="G6" s="46"/>
-      <c r="H6" s="34" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-      <c r="I6" s="54" t="inlineStr">
-        <is>
-          <t>Safrican Just Funeral [3000] is not a valid name Make sure that it does not include invalid characters or punctuation and that it is not too long</t>
-        </is>
-      </c>
-      <c r="J6" s="50" t="inlineStr">
-        <is>
-          <t>21/02/2022 10:41:37</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:10" ht="43" customHeight="1" x14ac:dyDescent="0.35" outlineLevel="0" r="7">
+      <c r="H6" s="34" t="s">
+        <v>307</v>
+      </c>
+      <c r="I6" s="54" t="s">
+        <v>308</v>
+      </c>
+      <c r="J6" s="50" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="43" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="37" t="s">
         <v>282</v>
       </c>
@@ -2351,36 +2415,24 @@
         <v>195</v>
       </c>
       <c r="D7" s="37"/>
-      <c r="E7" s="37" t="inlineStr">
-        <is>
-          <t>Safrican Provide and Protect Plan (4000)</t>
-        </is>
+      <c r="E7" s="37" t="s">
+        <v>311</v>
       </c>
       <c r="F7" s="37" t="s">
         <v>207</v>
       </c>
       <c r="G7" s="46"/>
-      <c r="H7" s="34" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-      <c r="I7" s="54" t="inlineStr">
-        <is>
-          <t>unexpected alert open: Alert text : There has been an error submitting your page
-Ensure that you have:
-  - Specified all mandatory fields
-  - Specified all fields using the correct format
-Hover over the highlighted controls for a description of the e</t>
-        </is>
-      </c>
-      <c r="J7" s="35" t="inlineStr">
-        <is>
-          <t>21/02/2022 10:42:56</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:10" ht="29" x14ac:dyDescent="0.35" outlineLevel="0" r="8">
+      <c r="H7" s="34" t="s">
+        <v>307</v>
+      </c>
+      <c r="I7" s="54" t="s">
+        <v>312</v>
+      </c>
+      <c r="J7" s="35" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="37" t="s">
         <v>294</v>
       </c>
@@ -2391,28 +2443,22 @@
         <v>196</v>
       </c>
       <c r="D8" s="37"/>
-      <c r="E8" s="37" t="inlineStr">
-        <is>
-          <t>Safrican Just Funeral (3000)</t>
-        </is>
+      <c r="E8" s="37" t="s">
+        <v>302</v>
       </c>
       <c r="F8" s="37" t="s">
         <v>207</v>
       </c>
       <c r="G8" s="46"/>
-      <c r="H8" s="33" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
+      <c r="H8" s="33" t="s">
+        <v>303</v>
       </c>
       <c r="I8" s="53"/>
-      <c r="J8" s="42" t="inlineStr">
-        <is>
-          <t>21/02/2022 10:44:25</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:10" ht="29" x14ac:dyDescent="0.35" outlineLevel="0" r="9">
+      <c r="J8" s="42" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="37" t="s">
         <v>294</v>
       </c>
@@ -2423,28 +2469,22 @@
         <v>198</v>
       </c>
       <c r="D9" s="37"/>
-      <c r="E9" s="37" t="inlineStr">
-        <is>
-          <t>Safrican Just Funeral (3000)</t>
-        </is>
+      <c r="E9" s="37" t="s">
+        <v>302</v>
       </c>
       <c r="F9" s="37" t="s">
         <v>207</v>
       </c>
       <c r="G9" s="46"/>
-      <c r="H9" s="33" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
+      <c r="H9" s="33" t="s">
+        <v>303</v>
       </c>
       <c r="I9" s="53"/>
-      <c r="J9" s="27" t="inlineStr">
-        <is>
-          <t>21/02/2022 10:46:29</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:10" ht="29" x14ac:dyDescent="0.35" outlineLevel="0" r="10">
+      <c r="J9" s="27" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="37" t="s">
         <v>295</v>
       </c>
@@ -2455,36 +2495,24 @@
         <v>197</v>
       </c>
       <c r="D10" s="37"/>
-      <c r="E10" s="37" t="inlineStr">
-        <is>
-          <t>Safrican Just Funeral (3000)</t>
-        </is>
+      <c r="E10" s="37" t="s">
+        <v>302</v>
       </c>
       <c r="F10" s="37" t="s">
         <v>207</v>
       </c>
       <c r="G10" s="46"/>
-      <c r="H10" s="34" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-      <c r="I10" s="54" t="inlineStr">
-        <is>
-          <t>unexpected alert open: Alert text : There has been an error submitting your page
-Ensure that you have:
-  - Specified all mandatory fields
-  - Specified all fields using the correct format
-Hover over the highlighted controls for a description of the e</t>
-        </is>
-      </c>
-      <c r="J10" s="36" t="inlineStr">
-        <is>
-          <t>21/02/2022 10:48:41</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:10" ht="29" x14ac:dyDescent="0.35" outlineLevel="0" r="11">
+      <c r="H10" s="34" t="s">
+        <v>307</v>
+      </c>
+      <c r="I10" s="54" t="s">
+        <v>312</v>
+      </c>
+      <c r="J10" s="36" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="37" t="s">
         <v>295</v>
       </c>
@@ -2495,28 +2523,22 @@
         <v>199</v>
       </c>
       <c r="D11" s="37"/>
-      <c r="E11" s="37" t="inlineStr">
-        <is>
-          <t>Safrican Just Funeral (3000)</t>
-        </is>
+      <c r="E11" s="37" t="s">
+        <v>302</v>
       </c>
       <c r="F11" s="37" t="s">
         <v>207</v>
       </c>
       <c r="G11" s="46"/>
-      <c r="H11" s="34" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
+      <c r="H11" s="34" t="s">
+        <v>303</v>
       </c>
       <c r="I11" s="54"/>
-      <c r="J11" s="36" t="inlineStr">
-        <is>
-          <t>21/02/2022 10:49:40</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:10" ht="29" x14ac:dyDescent="0.35" outlineLevel="0" r="12">
+      <c r="J11" s="36" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="37" t="s">
         <v>297</v>
       </c>
@@ -2527,33 +2549,24 @@
         <v>201</v>
       </c>
       <c r="D12" s="37"/>
-      <c r="E12" s="37" t="inlineStr">
-        <is>
-          <t>Safrican Just Funeral (3000)</t>
-        </is>
+      <c r="E12" s="37" t="s">
+        <v>302</v>
       </c>
       <c r="F12" s="37" t="s">
         <v>207</v>
       </c>
       <c r="G12" s="46"/>
-      <c r="H12" s="34" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-      <c r="I12" s="54" t="inlineStr">
-        <is>
-          <t>no such element: Unable to locate element: method:xpathselector://*[id=CntContentsDiv9]/table/tbody/tr[2]/td[4]
-  (Session info: chrome=970469271)</t>
-        </is>
-      </c>
-      <c r="J12" s="36" t="inlineStr">
-        <is>
-          <t>21/02/2022 10:51:14</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="13">
+      <c r="H12" s="34" t="s">
+        <v>307</v>
+      </c>
+      <c r="I12" s="54" t="s">
+        <v>318</v>
+      </c>
+      <c r="J12" s="36" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A13" s="37" t="s">
         <v>283</v>
       </c>
@@ -2564,33 +2577,24 @@
         <v>200</v>
       </c>
       <c r="D13" s="37"/>
-      <c r="E13" s="37" t="inlineStr">
-        <is>
-          <t>Safrican Just Funeral (3000)</t>
-        </is>
+      <c r="E13" s="37" t="s">
+        <v>302</v>
       </c>
       <c r="F13" s="37" t="s">
         <v>207</v>
       </c>
       <c r="G13" s="46"/>
-      <c r="H13" s="34" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-      <c r="I13" s="54" t="inlineStr">
-        <is>
-          <t>no such element: Unable to locate element: method:xpathselector://*[id=CntContentsDiv9]/table/tbody/tr[2]/td[4]
-  (Session info: chrome=970469271)</t>
-        </is>
-      </c>
-      <c r="J13" s="36" t="inlineStr">
-        <is>
-          <t>21/02/2022 10:52:47</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="14">
+      <c r="H13" s="34" t="s">
+        <v>307</v>
+      </c>
+      <c r="I13" s="54" t="s">
+        <v>318</v>
+      </c>
+      <c r="J13" s="36" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="37" t="s">
         <v>283</v>
       </c>
@@ -2601,28 +2605,22 @@
         <v>202</v>
       </c>
       <c r="D14" s="47"/>
-      <c r="E14" s="47" t="inlineStr">
-        <is>
-          <t>Safrican Just Funeral (3000)</t>
-        </is>
+      <c r="E14" s="47" t="s">
+        <v>302</v>
       </c>
       <c r="F14" s="47" t="s">
         <v>207</v>
       </c>
       <c r="G14" s="51"/>
-      <c r="H14" s="33" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
+      <c r="H14" s="33" t="s">
+        <v>303</v>
       </c>
       <c r="I14" s="53"/>
-      <c r="J14" s="49" t="inlineStr">
-        <is>
-          <t>21/02/2022 10:54:22</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="15">
+      <c r="J14" s="49" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A15" s="37" t="s">
         <v>284</v>
       </c>
@@ -2633,33 +2631,24 @@
         <v>203</v>
       </c>
       <c r="D15" s="37"/>
-      <c r="E15" s="37" t="inlineStr">
-        <is>
-          <t>Safrican Serenity Funeral Premium (1000)</t>
-        </is>
+      <c r="E15" s="37" t="s">
+        <v>322</v>
       </c>
       <c r="F15" s="37" t="s">
         <v>208</v>
       </c>
       <c r="G15" s="46"/>
-      <c r="H15" s="33" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-      <c r="I15" s="53" t="inlineStr">
-        <is>
-          <t>unexpected alert open: Alert text : The same policy payer was found with another employee number Would you like to update the employee number?
-  (Session info: chrome=970469271)</t>
-        </is>
-      </c>
-      <c r="J15" s="49" t="inlineStr">
-        <is>
-          <t>21/02/2022 10:55:43</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:10" ht="29" x14ac:dyDescent="0.35" outlineLevel="0" r="16">
+      <c r="H15" s="33" t="s">
+        <v>307</v>
+      </c>
+      <c r="I15" s="53" t="s">
+        <v>323</v>
+      </c>
+      <c r="J15" s="49" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A16" s="64" t="s">
         <v>301</v>
       </c>
@@ -2670,36 +2659,24 @@
         <v>206</v>
       </c>
       <c r="D16" s="47"/>
-      <c r="E16" s="47" t="inlineStr">
-        <is>
-          <t>Safrican Just Funeral (3000)</t>
-        </is>
+      <c r="E16" s="47" t="s">
+        <v>302</v>
       </c>
       <c r="F16" s="47" t="s">
         <v>208</v>
       </c>
       <c r="G16" s="46"/>
-      <c r="H16" s="33" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-      <c r="I16" s="53" t="inlineStr">
-        <is>
-          <t>  String lengths are both 72 Strings differ at index 11_x000d_
-  Expected: tstsafricancoza/web/wspd_cgish/WService=wsb_ilrtst/runw?_x000d_
-  But was:  intsafricancoza/web/wspd_cgish/WService=wsb_ilrint/runw?_x000d_
-  --------------^_x000d_
-</t>
-        </is>
-      </c>
-      <c r="J16" s="49" t="inlineStr">
-        <is>
-          <t>21/02/2022 10:56:41</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:10" x14ac:dyDescent="0.35" outlineLevel="0" r="17">
+      <c r="H16" s="33" t="s">
+        <v>307</v>
+      </c>
+      <c r="I16" s="53" t="s">
+        <v>325</v>
+      </c>
+      <c r="J16" s="49" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A17" s="58" t="s">
         <v>296</v>
       </c>
@@ -2710,33 +2687,24 @@
         <v>204</v>
       </c>
       <c r="D17" s="59"/>
-      <c r="E17" s="59" t="inlineStr">
-        <is>
-          <t>Safrican Serenity Funeral (2000)</t>
-        </is>
+      <c r="E17" s="59" t="s">
+        <v>327</v>
       </c>
       <c r="F17" s="59" t="s">
         <v>208</v>
       </c>
       <c r="G17" s="60"/>
-      <c r="H17" s="61" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-      <c r="I17" s="62" t="inlineStr">
-        <is>
-          <t>no such element: Unable to locate element: method:css selectorselector:#t0_749
-  (Session info: chrome=970469271)</t>
-        </is>
-      </c>
-      <c r="J17" s="63" t="inlineStr">
-        <is>
-          <t>21/02/2022 10:58:04</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:10" ht="29" x14ac:dyDescent="0.35" outlineLevel="0" r="18">
+      <c r="H17" s="61" t="s">
+        <v>307</v>
+      </c>
+      <c r="I17" s="62" t="s">
+        <v>328</v>
+      </c>
+      <c r="J17" s="63" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="58" t="s">
         <v>286</v>
       </c>
@@ -2747,25 +2715,19 @@
         <v>205</v>
       </c>
       <c r="D18" s="59"/>
-      <c r="E18" s="59" t="inlineStr">
-        <is>
-          <t>Safrican Serenity Funeral (2000)</t>
-        </is>
+      <c r="E18" s="59" t="s">
+        <v>327</v>
       </c>
       <c r="F18" s="59" t="s">
         <v>207</v>
       </c>
       <c r="G18" s="60"/>
-      <c r="H18" s="61" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
+      <c r="H18" s="61" t="s">
+        <v>303</v>
       </c>
       <c r="I18" s="62"/>
-      <c r="J18" s="63" t="inlineStr">
-        <is>
-          <t>21/02/2022 10:59:36</t>
-        </is>
+      <c r="J18" s="63" t="s">
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -3075,8 +3037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F12AD877-0D36-4EA9-9659-038739FDFBD2}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>